<commit_message>
Insurance Dispatcher Completed Everything.
</commit_message>
<xml_diff>
--- a/Data/Input/Insurance_Claims_Input_21-05-2025.xlsx
+++ b/Data/Input/Insurance_Claims_Input_21-05-2025.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5b498711e3aabb8c/Documents/UiPath/Insurance_Claim_Dispatcher/Data/Input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="38" documentId="13_ncr:1_{C8CB35C6-9866-4EDC-ADFC-9D1556290443}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8AAF860F-E6E4-4433-B90B-65C7B4290589}"/>
+  <xr:revisionPtr revIDLastSave="44" documentId="13_ncr:1_{C8CB35C6-9866-4EDC-ADFC-9D1556290443}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{59DDC7D9-8236-4E4B-A80D-309E647F8C4A}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="28">
   <si>
     <t>Claim ID</t>
   </si>
@@ -91,13 +91,19 @@
     <t>CLM1007</t>
   </si>
   <si>
-    <t>Correct Data 2</t>
-  </si>
-  <si>
     <t>CLM1008</t>
   </si>
   <si>
-    <t>Correct Data 3</t>
+    <t>Auto</t>
+  </si>
+  <si>
+    <t>Rejected Claim</t>
+  </si>
+  <si>
+    <t>Manual Review</t>
+  </si>
+  <si>
+    <t>Random</t>
   </si>
 </sst>
 </file>
@@ -180,6 +186,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -472,7 +482,7 @@
   <dimension ref="A1:O4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -595,10 +605,10 @@
         <v>19</v>
       </c>
       <c r="C3" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D3" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="E3" s="2">
         <v>45854</v>
@@ -636,13 +646,13 @@
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B4" t="s">
         <v>19</v>
       </c>
       <c r="C4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D4" t="s">
         <v>15</v>
@@ -657,7 +667,7 @@
         <v>16</v>
       </c>
       <c r="H4" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="I4">
         <v>124894</v>

</xml_diff>